<commit_message>
Uapdate Flink CalculateResource Summary in Knowledge.xlxs
</commit_message>
<xml_diff>
--- a/src/main/resources/Knowledge.xlsx
+++ b/src/main/resources/Knowledge.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Flink" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
     <sheet name="Spark深入" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
+    <sheet name="Flink资源管理" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="90">
   <si>
     <t>后备干部项目管理与经营——销售项目经营管理作业流程介绍</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -375,12 +376,214 @@
 允许把XML配置的某些参数配置到properties文件中</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Task Slot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SlotSharingGroup &amp;
+ CoLocationGroup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>总结</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Flink
+资源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Flink 如何对计算资源进行管理和隔离</t>
+  </si>
+  <si>
+    <t>如何将计算资源利用率最大化</t>
+  </si>
+  <si>
+    <t>Job 如何在集群中运行</t>
+  </si>
+  <si>
+    <t>为了更高效地分布式执行，Flink会尽可能地将operator的subtask链接（chain）在一起形成task。每个task在一个线程中执行。将operators链接成task是非常有效的优化：它能减少线程之间的切换，减少消息的序列化/反序列化，减少数据在缓冲区的交换，减少了延迟的同时提高整体的吞吐量。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt;-----&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Source并行度为1，FlatMap、KeyAggregation、Sink并行度均为2，最终以5个并行的线程来执行的优化过程。</t>
+  </si>
+  <si>
+    <t>其条件还是很苛刻的：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>将KeyAggregation和Sink两个operator进行了合并，因为这两个合并后并不会改变整体的拓扑结构。但是，并不是任意两个 operator 就能 chain 一起的。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.上下游的并行度一致
+2.下游节点的入度为1 （也就是说下游节点没有来自其他节点的输入）
+3.上下游节点都在同一个 slot group 中（下面会解释 slot group）
+4.下游节点的 chain 策略为 ALWAYS（可以与上下游链接，map、flatmap、filter等默认是ALWAYS）
+5.上游节点的 chain 策略为 ALWAYS 或 HEAD（只能与下游链接，不能与上游链接，Source默认是HEAD）
+6.两个节点间数据分区方式是 forward（参考理解数据流的分区）
+7.用户没有禁用 chain</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Operator chain的行为</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>可以通过编程API中进行指定</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>可以通过在DataStream的operator后面（如someStream.map(..))调用startNewChain()来指示从该operator开始一个新的chain（与前面截断，不会被chain到前面）。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>或者调用disableChaining()来指示该operator不参与chaining（不会与前后的operator chain一起）。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在底层，这两个方法都是通过调整operator的 chain 策略（HEAD、NEVER）来实现的。另外，也可以通过调用StreamExecutionEnvironment.disableOperatorChaining()来全局禁用chaining。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Operator Chains</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Operator Chains</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>例子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>原理与实现</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Flink是如何将多个 operators chain在一起的呢？
+chain在一起的operators是如何作为一个整体被执行的呢？
+它们之间的数据流又是如何避免了序列化/反序列化以及网络传输的呢？
+下图展示了operators chain的内部实现：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>如上图所示，Flink内部是通过OperatorChain这个类来将多个operator链在一起形成一个新的operator。OperatorChain形成的框框就像一个黑盒，Flink 无需知道黑盒中有多少个ChainOperator、数据在chain内部是怎么流动的，只需要将input数据交给 HeadOperator 就可以了，这就使得OperatorChain在行为上与普通的operator无差别，上面的OperaotrChain就可以看做是一个入度为1，出度为2的operator。
+所以在实现中，对外可见的只有HeadOperator，以及与外部连通的实线输出，这些输出对应了JobGraph中的JobEdge，在底层通过RecordWriterOutput来实现。
+另外，框中的虚线是operator chain内部的数据流，这个流内的数据不会经过序列化/反序列化、网络传输，而是直接将消息对象传递给下游的 ChainOperator 处理，这是性能提升的关键点，在底层是通过 ChainingOutput 实现的。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>源码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>注：HeadOperator和ChainOperator并不是具体的数据结构，前者指代chain中的第一个operator，后者指代chain中其余的operator，它们实际上都是StreamOperator。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TaskManager 是一个 JVM 进程，并会以独立的线程来执行一个task或多个subtask。为了控制一个 TaskManager 能接受多少个 task，Flink 提出了 Task Slot 的概念。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Flink 中的计算资源通过 Task Slot 来定义。每个 task slot 代表了 TaskManager 的一个固定大小的资源子集。例如，一个拥有3个slot的 TaskManager，会将其管理的内存平均分成三分分给各个 slot。将资源 slot 化意味着来自不同job的task不会为了内存而竞争，而是每个task都拥有一定数量的内存储备。需要注意的是，这里不会涉及到CPU的隔离，slot目前仅仅用来隔离task的内存。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>通过调整 task slot 的数量，用户可以定义task之间是如何相互隔离的。每个 TaskManager 有一个slot，也就意味着每个task运行在独立的 JVM 中。每个 TaskManager 有多个slot的话，也就是说多个task运行在同一个JVM中。而在同一个JVM进程中的task，可以共享TCP连接（基于多路复用）和心跳消息，可以减少数据的网络传输。也能共享一些数据结构，一定程度上减少了每个task的消耗。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每一个 TaskManager 会拥有一个或多个的 task slot，每个 slot 都能跑由多个连续 task 组成的一个 pipeline，比如 MapFunction 的第n个并行实例和 ReduceFunction 的第n个并行实例可以组成一个 pipeline。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5个Task可能会在TaskManager的slots中如下图分布，2个TaskManager，每个有3个slot：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SlotSharingGroup 与 CoLocationGroup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Task Slot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>默认情况下，Flink 允许subtasks共享slot，条件是它们都来自同一个Job的不同task的subtask。结果可能一个slot持有该job的整个pipeline。允许slot共享有以下两点好处：
+1.Flink 集群所需的task slots数与job中最高的并行度一致。也就是说我们不需要再去计算一个程序总共会起多少个task了。
+2.更容易获得更充分的资源利用。如果没有slot共享，那么非密集型操作source/flatmap就会占用同密集型操作 keyAggregation/sink 一样多的资源。如果有slot共享，将基线的2个并行度增加到6个，能充分利用slot资源，同时保证每个TaskManager能平均分配到重的subtasks。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>我们将 WordCount 的并行度从之前的2个增加到6个（Source并行度仍为1），并开启slot共享（所有operator都在default共享组），将得到如上图所示的slot分布图。首先，我们不用去计算这个job会其多少个task，总之该任务最终会占用6个slots（最高并行度为6）。其次，我们可以看到密集型操作 keyAggregation/sink 被平均地分配到各个 TaskManager。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SlotSharingGroup是Flink中用来实现slot共享的类，它尽可能地让subtasks共享一个slot。相应的，还有一个 CoLocationGroup 类用来强制将 subtasks 放到同一个 slot 中。CoLocationGroup主要用于迭代流中，用来保证迭代头与迭代尾的第i个subtask能被调度到同一个TaskManager上。这里我们不会详细讨论CoLocationGroup的实现细节。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>怎么判断operator属于哪个 slot 共享组呢？默认情况下，所有的operator都属于默认的共享组default，也就是说默认情况下所有的operator都是可以共享一个slot的。而当所有input operators具有相同的slot共享组时，该operator会继承这个共享组。最后，为了防止不合理的共享，用户也能通过API来强制指定operator的共享组，比如：someStream.filter(...).slotSharingGroup("group1");就强制指定了filter的slot共享组为group1。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>那么多个tasks（或者说operators）是如何共享slot的呢？
+用来定义计算资源的slot的类图：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>抽象类Slot定义了该槽位属于哪个TaskManager（instance）的第几个槽位（slotNumber），属于哪个Job（jobID）等信息。最简单的情况下，一个slot只持有一个task，也就是SimpleSlot的实现。复杂点的情况，一个slot能共享给多个task使用，也就是SharedSlot的实现。SharedSlot能包含其他的SharedSlot，也能包含SimpleSlot。所以一个SharedSlot能定义出一棵slots树。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>接下来我们来看看 Flink 为subtask分配slot的过程。关于Flink调度，有两个非常重要的原则我们必须知道：
+1.同一个operator的各个subtask是不能呆在同一个SharedSlot中的，例如FlatMap[1]和FlatMap[2]是不能在同一个SharedSlot中的。
+2.Flink是按照拓扑顺序从Source一个个调度到Sink的。例如WordCount（Source并行度为1，其他并行度为2），那么调度的顺序依次是：Source -&gt; FlatMap[1] -&gt; FlatMap[2] -&gt; KeyAgg-&gt;Sink[1] -&gt; KeyAgg-&gt;Sink[2]。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>假设现在有2个TaskManager，每个只有1个slot（为简化问题），那么分配slot的过程如图所示：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>注：图中 SharedSlot 与 SimpleSlot 后带的括号中的数字代表槽位号（slotNumber）
+1.为Source分配slot。首先，我们从TaskManager1中分配出一个SharedSlot。并从SharedSlot中为Source分配出一个SimpleSlot。如上图中的①和②。
+2.为FlatMap[1]分配slot。目前已经有一个SharedSlot，则从该SharedSlot中分配出一个SimpleSlot用来部署FlatMap[1]。如上图中的③。
+为FlatMap[2]分配slot。由于TaskManager1的SharedSlot中已经有同operator的FlatMap[1]了，我们只能3.分配到其他SharedSlot中去。从TaskManager2中分配出一个SharedSlot，并从该SharedSlot中为FlatMap[2]分配出一个SimpleSlot。如上图的④和⑤。
+4.为Key-&gt;Sink[1]分配slot。目前两个SharedSlot都符合条件，从TaskManager1的SharedSlot中分配出一个SimpleSlot用来部署Key-&gt;Sink[1]。如上图中的⑥。
+5.为Key-&gt;Sink[2]分配slot。TaskManager1的SharedSlot中已经有同operator的Key-&gt;Sink[1]了，则只能选择另一个SharedSlot中分配出一个SimpleSlot用来部署Key-&gt;Sink[2]。如上图中的⑦。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最后Source、FlatMap[1]、Key-&gt;Sink[1]这些subtask都会部署到TaskManager1的唯一一个slot中，并启动对应的线程。FlatMap[2]、Key-&gt;Sink[2]这些subtask都会被部署到TaskManager2的唯一一个slot中，并启动对应的线程。从而实现了slot共享。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>总结</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主要介绍了Flink中计算资源的相关概念以及原理实现。
+最核心的是 Task Slot，每个slot能运行一个或多个task。
+为了拓扑更高效地运行，Flink提出了Chaining，尽可能地将operators chain在一起作为一个task来处理。
+为了资源更充分的利用，Flink又提出了SlotSharingGroup，尽可能地让多个task共享一个slot。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -453,8 +656,14 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -482,6 +691,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF0099FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -645,10 +866,19 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -712,28 +942,70 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -742,55 +1014,70 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -809,6 +1096,51 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>286867</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 1" descr="http://img3.tbcdn.cn/5476e8b07b923/TB18Gv5JFXXXXcDXXXXXXXXXXXX?spm=5176.100239.0.0.9lgfsK"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11277600" y="895350"/>
+          <a:ext cx="5087467" cy="4238625"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1041,6 +1373,369 @@
           <a:tailEnd type="none" w="med" len="med"/>
         </a:ln>
         <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>685799</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>146613</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 1" descr="http://img3.tbcdn.cn/5476e8b07b923/TB18Gv5JFXXXXcDXXXXXXXXXXXX?spm=5176.100239.0.0.9lgfsK"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="685799" y="1304924"/>
+          <a:ext cx="6328339" cy="4419601"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2049" name="AutoShape 1" descr="http://img3.tbcdn.cn/5476e8b07b923/TB1cFbJJFXXXXaIXVXXXXXXXXXX?spm=5176.100239.0.0.9lgfsK"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6867525" y="1914525"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>685799</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>352424</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>352424</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2051" name="AutoShape 3" descr="http://img3.tbcdn.cn/5476e8b07b923/TB1cFbJJFXXXXaIXVXXXXXXXXXX"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8924924" y="4486274"/>
+          <a:ext cx="1724025" cy="1724025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>504825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>57149</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>56310</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="图片 6" descr="TB1cFbJJFXXXXaIXVXXXXXXXXXX.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7800975" y="1733550"/>
+          <a:ext cx="6667499" cy="3323385"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>139575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2052" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7648575" y="7800975"/>
+          <a:ext cx="6667500" cy="3701925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>228828</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2054" name="Picture 6" descr="http://img3.tbcdn.cn/5476e8b07b923/TB1Q4zUJFXXXXXnXVXXXXXXXXXX?spm=5176.100239.0.0.w7Y37a"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="685800" y="12944476"/>
+          <a:ext cx="6410553" cy="2419350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>241812</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2055" name="Picture 7" descr="http://img3.tbcdn.cn/5476e8b07b923/TB1VTj4JFXXXXX8XFXXXXXXXXXX?spm=5176.100239.0.0.w7Y37a"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="685801" y="17278350"/>
+          <a:ext cx="6423536" cy="3019425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>354921</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2056" name="Picture 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7908246" y="18240376"/>
+          <a:ext cx="6198279" cy="2886074"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>613503</xdr:colOff>
+      <xdr:row>147</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2057" name="Picture 9" descr="http://img3.tbcdn.cn/5476e8b07b923/TB1TM_3JFXXXXb8XVXXXXXXXXXX?spm=5176.100239.0.0.w7Y37a"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7553325" y="23726776"/>
+          <a:ext cx="6785703" cy="6057899"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1333,172 +2028,578 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:K13"/>
+  <dimension ref="B2:T53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5:T52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="2" max="2" width="13.75" customWidth="1"/>
+    <col min="3" max="3" width="26.25" customWidth="1"/>
+    <col min="7" max="7" width="17.875" customWidth="1"/>
+    <col min="8" max="8" width="18.125" customWidth="1"/>
+    <col min="20" max="20" width="9" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:11">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="2:18" ht="15">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="10" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="12"/>
-    </row>
-    <row r="3" spans="2:11">
-      <c r="B3" s="4"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="15"/>
-    </row>
-    <row r="4" spans="2:11">
-      <c r="B4" s="4"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="15"/>
-    </row>
-    <row r="5" spans="2:11">
-      <c r="B5" s="4"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="15"/>
-    </row>
-    <row r="6" spans="2:11">
-      <c r="B6" s="4"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="15"/>
-    </row>
-    <row r="7" spans="2:11">
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="18"/>
-    </row>
-    <row r="8" spans="2:11">
-      <c r="B8" s="1"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="12"/>
-    </row>
-    <row r="9" spans="2:11">
-      <c r="B9" s="4"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="15"/>
-    </row>
-    <row r="10" spans="2:11">
-      <c r="B10" s="4"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="15"/>
-    </row>
-    <row r="11" spans="2:11">
-      <c r="B11" s="4"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="15"/>
-    </row>
-    <row r="12" spans="2:11">
-      <c r="B12" s="4"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="15"/>
-    </row>
-    <row r="13" spans="2:11">
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="18"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="15"/>
+      <c r="M2" s="53" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>53</v>
+      </c>
+      <c r="R2" s="53" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" ht="15">
+      <c r="B3" s="7"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="18"/>
+      <c r="M3" s="53" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18">
+      <c r="B4" s="7"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="18"/>
+    </row>
+    <row r="5" spans="2:18" ht="13.5" customHeight="1">
+      <c r="B5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="18"/>
+    </row>
+    <row r="6" spans="2:18" ht="3" hidden="1" customHeight="1">
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="18"/>
+    </row>
+    <row r="7" spans="2:18" hidden="1">
+      <c r="B7" s="10"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="21"/>
+    </row>
+    <row r="8" spans="2:18">
+      <c r="B8" s="4"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="15"/>
+    </row>
+    <row r="9" spans="2:18">
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="18"/>
+    </row>
+    <row r="10" spans="2:18">
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="18"/>
+    </row>
+    <row r="11" spans="2:18">
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="18"/>
+    </row>
+    <row r="12" spans="2:18">
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="18"/>
+    </row>
+    <row r="13" spans="2:18">
+      <c r="B13" s="10"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="21"/>
+    </row>
+    <row r="15" spans="2:18" ht="29.25" customHeight="1">
+      <c r="B15" s="51" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="50" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="55"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="55"/>
+      <c r="H15" s="55"/>
+    </row>
+    <row r="16" spans="2:18" ht="26.25" customHeight="1">
+      <c r="B16" s="50"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="55"/>
+      <c r="G16" s="55"/>
+      <c r="H16" s="55"/>
+    </row>
+    <row r="17" spans="2:20" ht="27.75" customHeight="1">
+      <c r="B17" s="50"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="55"/>
+      <c r="G17" s="55"/>
+      <c r="H17" s="55"/>
+    </row>
+    <row r="18" spans="2:20">
+      <c r="B18" s="50"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="49"/>
+      <c r="H18" s="49"/>
+    </row>
+    <row r="19" spans="2:20">
+      <c r="B19" s="50"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="52"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="49"/>
+      <c r="H19" s="49"/>
+    </row>
+    <row r="20" spans="2:20">
+      <c r="B20" s="50"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="49"/>
+    </row>
+    <row r="21" spans="2:20">
+      <c r="B21" s="50"/>
+      <c r="C21" s="50"/>
+    </row>
+    <row r="22" spans="2:20">
+      <c r="B22" s="50"/>
+      <c r="C22" s="50"/>
+    </row>
+    <row r="23" spans="2:20">
+      <c r="B23" s="50"/>
+      <c r="C23" s="50" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="2:20">
+      <c r="B24" s="50"/>
+      <c r="C24" s="50"/>
+    </row>
+    <row r="25" spans="2:20">
+      <c r="B25" s="50"/>
+      <c r="C25" s="50"/>
+    </row>
+    <row r="26" spans="2:20">
+      <c r="B26" s="50"/>
+      <c r="C26" s="50"/>
+    </row>
+    <row r="27" spans="2:20">
+      <c r="B27" s="50"/>
+      <c r="C27" s="50"/>
+    </row>
+    <row r="28" spans="2:20">
+      <c r="B28" s="50"/>
+      <c r="C28" s="50"/>
+    </row>
+    <row r="29" spans="2:20">
+      <c r="B29" s="50"/>
+      <c r="C29" s="50"/>
+    </row>
+    <row r="30" spans="2:20" ht="31.5" customHeight="1">
+      <c r="B30" s="50"/>
+      <c r="C30" s="50"/>
+      <c r="M30" s="57" t="s">
+        <v>54</v>
+      </c>
+      <c r="N30" s="57"/>
+      <c r="O30" s="57"/>
+      <c r="P30" s="57"/>
+      <c r="Q30" s="57"/>
+      <c r="R30" s="57"/>
+      <c r="S30" s="57"/>
+      <c r="T30" s="57"/>
+    </row>
+    <row r="31" spans="2:20">
+      <c r="B31" s="50"/>
+      <c r="C31" s="50"/>
+    </row>
+    <row r="32" spans="2:20" ht="28.5" customHeight="1">
+      <c r="B32" s="50"/>
+      <c r="C32" s="50"/>
+      <c r="M32" s="56" t="s">
+        <v>56</v>
+      </c>
+      <c r="N32" s="56"/>
+      <c r="O32" s="56"/>
+      <c r="P32" s="56"/>
+      <c r="Q32" s="56"/>
+      <c r="R32" s="56"/>
+      <c r="S32" s="56"/>
+      <c r="T32" s="56"/>
+    </row>
+    <row r="33" spans="2:20">
+      <c r="B33" s="50"/>
+      <c r="C33" s="50"/>
+    </row>
+    <row r="34" spans="2:20">
+      <c r="B34" s="50"/>
+      <c r="C34" s="50"/>
+      <c r="M34" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="N34" s="56"/>
+      <c r="O34" s="56"/>
+      <c r="P34" s="56"/>
+      <c r="Q34" s="56"/>
+      <c r="R34" s="56"/>
+      <c r="S34" s="56"/>
+      <c r="T34" s="56"/>
+    </row>
+    <row r="35" spans="2:20">
+      <c r="B35" s="50"/>
+      <c r="C35" s="50"/>
+      <c r="M35" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="N35" s="55"/>
+      <c r="O35" s="55"/>
+      <c r="P35" s="55"/>
+      <c r="Q35" s="55"/>
+      <c r="R35" s="55"/>
+      <c r="S35" s="55"/>
+      <c r="T35" s="55"/>
+    </row>
+    <row r="36" spans="2:20">
+      <c r="B36" s="50"/>
+      <c r="C36" s="50"/>
+      <c r="M36" s="55"/>
+      <c r="N36" s="55"/>
+      <c r="O36" s="55"/>
+      <c r="P36" s="55"/>
+      <c r="Q36" s="55"/>
+      <c r="R36" s="55"/>
+      <c r="S36" s="55"/>
+      <c r="T36" s="55"/>
+    </row>
+    <row r="37" spans="2:20">
+      <c r="B37" s="50"/>
+      <c r="C37" s="51" t="s">
+        <v>46</v>
+      </c>
+      <c r="M37" s="55"/>
+      <c r="N37" s="55"/>
+      <c r="O37" s="55"/>
+      <c r="P37" s="55"/>
+      <c r="Q37" s="55"/>
+      <c r="R37" s="55"/>
+      <c r="S37" s="55"/>
+      <c r="T37" s="55"/>
+    </row>
+    <row r="38" spans="2:20">
+      <c r="B38" s="50"/>
+      <c r="C38" s="50"/>
+      <c r="M38" s="55"/>
+      <c r="N38" s="55"/>
+      <c r="O38" s="55"/>
+      <c r="P38" s="55"/>
+      <c r="Q38" s="55"/>
+      <c r="R38" s="55"/>
+      <c r="S38" s="55"/>
+      <c r="T38" s="55"/>
+    </row>
+    <row r="39" spans="2:20">
+      <c r="B39" s="50"/>
+      <c r="C39" s="50"/>
+      <c r="M39" s="55"/>
+      <c r="N39" s="55"/>
+      <c r="O39" s="55"/>
+      <c r="P39" s="55"/>
+      <c r="Q39" s="55"/>
+      <c r="R39" s="55"/>
+      <c r="S39" s="55"/>
+      <c r="T39" s="55"/>
+    </row>
+    <row r="40" spans="2:20">
+      <c r="B40" s="50"/>
+      <c r="C40" s="50"/>
+      <c r="M40" s="55"/>
+      <c r="N40" s="55"/>
+      <c r="O40" s="55"/>
+      <c r="P40" s="55"/>
+      <c r="Q40" s="55"/>
+      <c r="R40" s="55"/>
+      <c r="S40" s="55"/>
+      <c r="T40" s="55"/>
+    </row>
+    <row r="41" spans="2:20">
+      <c r="B41" s="50"/>
+      <c r="C41" s="50"/>
+      <c r="M41" s="55"/>
+      <c r="N41" s="55"/>
+      <c r="O41" s="55"/>
+      <c r="P41" s="55"/>
+      <c r="Q41" s="55"/>
+      <c r="R41" s="55"/>
+      <c r="S41" s="55"/>
+      <c r="T41" s="55"/>
+    </row>
+    <row r="42" spans="2:20" ht="42" customHeight="1">
+      <c r="B42" s="50"/>
+      <c r="C42" s="50"/>
+      <c r="M42" s="55"/>
+      <c r="N42" s="55"/>
+      <c r="O42" s="55"/>
+      <c r="P42" s="55"/>
+      <c r="Q42" s="55"/>
+      <c r="R42" s="55"/>
+      <c r="S42" s="55"/>
+      <c r="T42" s="55"/>
+    </row>
+    <row r="43" spans="2:20">
+      <c r="B43" s="50"/>
+      <c r="C43" s="50"/>
+    </row>
+    <row r="44" spans="2:20">
+      <c r="B44" s="50"/>
+      <c r="C44" s="50"/>
+      <c r="M44" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="N44" s="39"/>
+      <c r="O44" s="58" t="s">
+        <v>59</v>
+      </c>
+      <c r="P44" s="32"/>
+      <c r="Q44" s="32"/>
+      <c r="R44" s="32"/>
+      <c r="S44" s="32"/>
+      <c r="T44" s="32"/>
+    </row>
+    <row r="45" spans="2:20" ht="27" customHeight="1">
+      <c r="B45" s="50"/>
+      <c r="C45" s="51" t="s">
+        <v>47</v>
+      </c>
+      <c r="M45" s="39"/>
+      <c r="N45" s="39"/>
+      <c r="O45" s="59" t="s">
+        <v>60</v>
+      </c>
+      <c r="P45" s="39"/>
+      <c r="Q45" s="39"/>
+      <c r="R45" s="39"/>
+      <c r="S45" s="39"/>
+      <c r="T45" s="39"/>
+    </row>
+    <row r="46" spans="2:20">
+      <c r="B46" s="50"/>
+      <c r="C46" s="51"/>
+      <c r="M46" s="39"/>
+      <c r="N46" s="39"/>
+      <c r="O46" s="59"/>
+      <c r="P46" s="39"/>
+      <c r="Q46" s="39"/>
+      <c r="R46" s="39"/>
+      <c r="S46" s="39"/>
+      <c r="T46" s="39"/>
+    </row>
+    <row r="47" spans="2:20">
+      <c r="B47" s="50"/>
+      <c r="C47" s="51"/>
+      <c r="M47" s="39"/>
+      <c r="N47" s="39"/>
+      <c r="O47" s="59"/>
+      <c r="P47" s="39"/>
+      <c r="Q47" s="39"/>
+      <c r="R47" s="39"/>
+      <c r="S47" s="39"/>
+      <c r="T47" s="39"/>
+    </row>
+    <row r="48" spans="2:20">
+      <c r="B48" s="50"/>
+      <c r="C48" s="51"/>
+      <c r="M48" s="39"/>
+      <c r="N48" s="39"/>
+      <c r="O48" s="59" t="s">
+        <v>61</v>
+      </c>
+      <c r="P48" s="39"/>
+      <c r="Q48" s="39"/>
+      <c r="R48" s="39"/>
+      <c r="S48" s="39"/>
+      <c r="T48" s="39"/>
+    </row>
+    <row r="49" spans="2:20">
+      <c r="B49" s="50"/>
+      <c r="C49" s="51"/>
+      <c r="M49" s="39"/>
+      <c r="N49" s="39"/>
+      <c r="O49" s="59"/>
+      <c r="P49" s="39"/>
+      <c r="Q49" s="39"/>
+      <c r="R49" s="39"/>
+      <c r="S49" s="39"/>
+      <c r="T49" s="39"/>
+    </row>
+    <row r="50" spans="2:20">
+      <c r="B50" s="50"/>
+      <c r="C50" s="51"/>
+      <c r="M50" s="39"/>
+      <c r="N50" s="39"/>
+    </row>
+    <row r="51" spans="2:20" ht="27" customHeight="1">
+      <c r="B51" s="50"/>
+      <c r="C51" s="51"/>
+      <c r="M51" s="39"/>
+      <c r="N51" s="39"/>
+      <c r="O51" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="P51" s="39"/>
+      <c r="Q51" s="39"/>
+      <c r="R51" s="39"/>
+      <c r="S51" s="39"/>
+      <c r="T51" s="39"/>
+    </row>
+    <row r="52" spans="2:20" ht="27" customHeight="1">
+      <c r="B52" s="50"/>
+      <c r="C52" s="51"/>
+      <c r="M52" s="39"/>
+      <c r="N52" s="39"/>
+      <c r="O52" s="39"/>
+      <c r="P52" s="39"/>
+      <c r="Q52" s="39"/>
+      <c r="R52" s="39"/>
+      <c r="S52" s="39"/>
+      <c r="T52" s="39"/>
+    </row>
+    <row r="53" spans="2:20">
+      <c r="B53" s="50"/>
+      <c r="C53" s="51"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="20">
+    <mergeCell ref="M30:T30"/>
+    <mergeCell ref="M35:T42"/>
+    <mergeCell ref="M34:T34"/>
+    <mergeCell ref="M32:T32"/>
+    <mergeCell ref="M44:N52"/>
+    <mergeCell ref="O44:T44"/>
+    <mergeCell ref="O45:T47"/>
+    <mergeCell ref="O48:T49"/>
+    <mergeCell ref="O51:T52"/>
     <mergeCell ref="B2:F7"/>
     <mergeCell ref="G2:K7"/>
     <mergeCell ref="B8:F13"/>
     <mergeCell ref="G8:K13"/>
+    <mergeCell ref="C23:C36"/>
+    <mergeCell ref="C15:C22"/>
+    <mergeCell ref="C37:C44"/>
+    <mergeCell ref="B15:B53"/>
+    <mergeCell ref="C45:C53"/>
+    <mergeCell ref="D15:H17"/>
+    <mergeCell ref="D18:H20"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1512,23 +2613,23 @@
   <sheetData>
     <row r="1" spans="2:16" ht="36.75" customHeight="1"/>
     <row r="2" spans="2:16" ht="27" customHeight="1">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1552,340 +2653,340 @@
   <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="2" spans="2:11">
-      <c r="B2" s="1"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="12"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="15"/>
     </row>
     <row r="3" spans="2:11">
-      <c r="B3" s="4"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="15"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="18"/>
     </row>
     <row r="4" spans="2:11">
-      <c r="B4" s="4"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="15"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="18"/>
     </row>
     <row r="5" spans="2:11">
-      <c r="B5" s="4"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="15"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="18"/>
     </row>
     <row r="6" spans="2:11">
-      <c r="B6" s="4"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="15"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="18"/>
     </row>
     <row r="7" spans="2:11">
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="18"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="21"/>
     </row>
     <row r="8" spans="2:11">
-      <c r="B8" s="1"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="12"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="15"/>
     </row>
     <row r="9" spans="2:11">
-      <c r="B9" s="4"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="15"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="18"/>
     </row>
     <row r="10" spans="2:11">
-      <c r="B10" s="4"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="15"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="18"/>
     </row>
     <row r="11" spans="2:11">
-      <c r="B11" s="4"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="15"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="18"/>
     </row>
     <row r="12" spans="2:11">
-      <c r="B12" s="4"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="15"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="18"/>
     </row>
     <row r="13" spans="2:11">
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="18"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="21"/>
     </row>
     <row r="14" spans="2:11">
-      <c r="B14" s="1"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="12"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="15"/>
     </row>
     <row r="15" spans="2:11">
-      <c r="B15" s="4"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="15"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="18"/>
     </row>
     <row r="16" spans="2:11">
-      <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="18"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="21"/>
     </row>
     <row r="17" spans="2:11">
-      <c r="B17" s="1"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="12"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="15"/>
     </row>
     <row r="18" spans="2:11">
-      <c r="B18" s="4"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="15"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="18"/>
     </row>
     <row r="19" spans="2:11">
-      <c r="B19" s="7"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="18"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="21"/>
     </row>
     <row r="20" spans="2:11">
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="21"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
     </row>
     <row r="21" spans="2:11">
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="21"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24"/>
     </row>
     <row r="22" spans="2:11">
-      <c r="B22" s="20"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="21"/>
-      <c r="K22" s="21"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
     </row>
     <row r="23" spans="2:11">
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="21"/>
-      <c r="J23" s="21"/>
-      <c r="K23" s="21"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
     </row>
     <row r="24" spans="2:11">
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="21"/>
-      <c r="J24" s="21"/>
-      <c r="K24" s="21"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24"/>
     </row>
     <row r="25" spans="2:11">
-      <c r="B25" s="20"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="21"/>
-      <c r="J25" s="21"/>
-      <c r="K25" s="21"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="24"/>
     </row>
     <row r="26" spans="2:11">
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21"/>
-      <c r="J26" s="21"/>
-      <c r="K26" s="21"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="24"/>
+      <c r="K26" s="24"/>
     </row>
     <row r="27" spans="2:11">
-      <c r="B27" s="20"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="21"/>
-      <c r="J27" s="21"/>
-      <c r="K27" s="21"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
+      <c r="K27" s="24"/>
     </row>
     <row r="28" spans="2:11">
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="21"/>
-      <c r="J28" s="21"/>
-      <c r="K28" s="21"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
+      <c r="K28" s="24"/>
     </row>
     <row r="29" spans="2:11">
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="21"/>
-      <c r="I29" s="21"/>
-      <c r="J29" s="21"/>
-      <c r="K29" s="21"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="24"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="24"/>
+      <c r="J29" s="24"/>
+      <c r="K29" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -1910,7 +3011,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:F60"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A30" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A6" workbookViewId="0">
       <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
@@ -1925,374 +3026,374 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="13.5" customHeight="1">
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="45" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="13.5" customHeight="1">
-      <c r="B3" s="48"/>
-      <c r="C3" s="36"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="46"/>
     </row>
     <row r="4" spans="2:6" ht="13.5" customHeight="1">
-      <c r="B4" s="48"/>
-      <c r="C4" s="36"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="46"/>
     </row>
     <row r="5" spans="2:6" ht="13.5" customHeight="1">
-      <c r="B5" s="48"/>
-      <c r="C5" s="36"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="46"/>
     </row>
     <row r="6" spans="2:6" ht="13.5" customHeight="1">
-      <c r="B6" s="48"/>
-      <c r="C6" s="36"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="46"/>
     </row>
     <row r="7" spans="2:6" ht="13.5" customHeight="1">
-      <c r="B7" s="48"/>
-      <c r="C7" s="36"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="46"/>
     </row>
     <row r="8" spans="2:6" ht="13.5" customHeight="1">
-      <c r="B8" s="48"/>
-      <c r="C8" s="36"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="46"/>
     </row>
     <row r="9" spans="2:6" ht="13.5" customHeight="1">
-      <c r="B9" s="48"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="23" t="s">
+      <c r="B9" s="28"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="32" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="13.5" customHeight="1">
-      <c r="B10" s="48"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="23"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="32"/>
     </row>
     <row r="11" spans="2:6" ht="13.5" customHeight="1">
-      <c r="B11" s="48"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="23"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="32"/>
     </row>
     <row r="12" spans="2:6" ht="13.5" customHeight="1">
-      <c r="B12" s="48"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="23"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="32"/>
     </row>
     <row r="13" spans="2:6" ht="13.5" customHeight="1">
-      <c r="B13" s="48"/>
-      <c r="C13" s="37" t="s">
+      <c r="B13" s="28"/>
+      <c r="C13" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="27" t="s">
+      <c r="D13" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="22"/>
+      <c r="F13" s="39"/>
     </row>
     <row r="14" spans="2:6" ht="13.5" customHeight="1">
-      <c r="B14" s="48"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
     </row>
     <row r="15" spans="2:6" ht="8.25" customHeight="1">
-      <c r="B15" s="48"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
     </row>
     <row r="16" spans="2:6" ht="13.5" hidden="1" customHeight="1">
-      <c r="B16" s="48"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
     </row>
     <row r="17" spans="2:6" ht="13.5" hidden="1" customHeight="1">
-      <c r="B17" s="48"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
     </row>
     <row r="18" spans="2:6" ht="3.75" customHeight="1">
-      <c r="B18" s="48"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
     </row>
     <row r="19" spans="2:6" ht="13.5" hidden="1" customHeight="1">
-      <c r="B19" s="48"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
     </row>
     <row r="20" spans="2:6" ht="13.5" hidden="1" customHeight="1">
-      <c r="B20" s="48"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="39"/>
+      <c r="F20" s="39"/>
     </row>
     <row r="21" spans="2:6" ht="13.5" customHeight="1">
-      <c r="B21" s="48"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="30" t="s">
+      <c r="B21" s="28"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="E21" s="23" t="s">
+      <c r="E21" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="F21" s="23"/>
+      <c r="F21" s="32"/>
     </row>
     <row r="22" spans="2:6" ht="13.5" customHeight="1">
-      <c r="B22" s="48"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="48"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
     </row>
     <row r="23" spans="2:6" ht="13.5" hidden="1" customHeight="1">
-      <c r="B23" s="48"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
     </row>
     <row r="24" spans="2:6" ht="9" customHeight="1">
-      <c r="B24" s="48"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="48"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="32"/>
     </row>
     <row r="25" spans="2:6" ht="13.5" hidden="1" customHeight="1">
-      <c r="B25" s="48"/>
-      <c r="C25" s="38"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="48"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
     </row>
     <row r="26" spans="2:6" ht="13.5" hidden="1" customHeight="1">
-      <c r="B26" s="48"/>
-      <c r="C26" s="38"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="48"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
     </row>
     <row r="27" spans="2:6" ht="13.5" customHeight="1">
-      <c r="B27" s="48"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="31" t="s">
+      <c r="B27" s="28"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="E27" s="22" t="s">
+      <c r="E27" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="F27" s="23"/>
+      <c r="F27" s="32"/>
     </row>
     <row r="28" spans="2:6" ht="13.5" customHeight="1">
-      <c r="B28" s="48"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="48"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
     </row>
     <row r="29" spans="2:6" ht="13.5" customHeight="1">
-      <c r="B29" s="48"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="48"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
     </row>
     <row r="30" spans="2:6" ht="13.5" customHeight="1">
-      <c r="B30" s="48"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="32" t="s">
+      <c r="B30" s="28"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E30" s="22" t="s">
+      <c r="E30" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="F30" s="23"/>
+      <c r="F30" s="32"/>
     </row>
     <row r="31" spans="2:6" ht="69" customHeight="1">
-      <c r="B31" s="48"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="32" t="s">
+      <c r="B31" s="28"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E31" s="22" t="s">
+      <c r="E31" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="F31" s="23"/>
+      <c r="F31" s="32"/>
     </row>
     <row r="32" spans="2:6" ht="74.25" customHeight="1">
-      <c r="B32" s="48"/>
-      <c r="C32" s="38"/>
-      <c r="D32" s="32" t="s">
+      <c r="B32" s="28"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E32" s="22" t="s">
+      <c r="E32" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="F32" s="23"/>
+      <c r="F32" s="32"/>
     </row>
     <row r="33" spans="2:6" ht="33.75" customHeight="1">
-      <c r="B33" s="48"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="33" t="s">
+      <c r="B33" s="28"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E33" s="26" t="s">
+      <c r="E33" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="F33" s="25"/>
+      <c r="F33" s="44"/>
     </row>
     <row r="34" spans="2:6" ht="39" customHeight="1">
-      <c r="B34" s="48"/>
-      <c r="C34" s="38"/>
-      <c r="D34" s="34" t="s">
+      <c r="B34" s="28"/>
+      <c r="C34" s="31"/>
+      <c r="D34" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E34" s="22"/>
-      <c r="F34" s="23"/>
+      <c r="E34" s="39"/>
+      <c r="F34" s="32"/>
     </row>
     <row r="35" spans="2:6" ht="15" customHeight="1">
-      <c r="B35" s="48"/>
-      <c r="C35" s="38"/>
-      <c r="D35" s="34" t="s">
+      <c r="B35" s="28"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E35" s="22"/>
-      <c r="F35" s="23"/>
+      <c r="E35" s="39"/>
+      <c r="F35" s="32"/>
     </row>
     <row r="36" spans="2:6" ht="69.75" customHeight="1">
-      <c r="B36" s="48"/>
-      <c r="C36" s="38"/>
-      <c r="D36" s="34" t="s">
+      <c r="B36" s="28"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E36" s="22" t="s">
+      <c r="E36" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="F36" s="23"/>
+      <c r="F36" s="32"/>
     </row>
     <row r="37" spans="2:6" ht="48" customHeight="1">
-      <c r="B37" s="48"/>
-      <c r="C37" s="38"/>
-      <c r="D37" s="34" t="s">
+      <c r="B37" s="28"/>
+      <c r="C37" s="31"/>
+      <c r="D37" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E37" s="22" t="s">
+      <c r="E37" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="F37" s="23"/>
+      <c r="F37" s="32"/>
     </row>
     <row r="38" spans="2:6" ht="92.25" customHeight="1">
-      <c r="B38" s="48"/>
-      <c r="C38" s="38"/>
-      <c r="D38" s="34" t="s">
+      <c r="B38" s="28"/>
+      <c r="C38" s="31"/>
+      <c r="D38" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E38" s="22" t="s">
+      <c r="E38" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="F38" s="23"/>
+      <c r="F38" s="32"/>
     </row>
     <row r="39" spans="2:6" ht="50.25" customHeight="1">
-      <c r="B39" s="48"/>
-      <c r="C39" s="38"/>
-      <c r="D39" s="34" t="s">
+      <c r="B39" s="28"/>
+      <c r="C39" s="31"/>
+      <c r="D39" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E39" s="22" t="s">
+      <c r="E39" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="F39" s="23"/>
+      <c r="F39" s="32"/>
     </row>
     <row r="40" spans="2:6" ht="95.25" customHeight="1">
-      <c r="B40" s="48"/>
-      <c r="C40" s="38"/>
-      <c r="D40" s="34" t="s">
+      <c r="B40" s="28"/>
+      <c r="C40" s="31"/>
+      <c r="D40" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E40" s="22" t="s">
+      <c r="E40" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="F40" s="23"/>
+      <c r="F40" s="32"/>
     </row>
     <row r="41" spans="2:6" ht="18" customHeight="1">
-      <c r="B41" s="48"/>
-      <c r="C41" s="40" t="s">
+      <c r="B41" s="28"/>
+      <c r="C41" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="D41" s="34" t="s">
+      <c r="D41" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E41" s="22" t="s">
+      <c r="E41" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="F41" s="23"/>
+      <c r="F41" s="32"/>
     </row>
     <row r="42" spans="2:6" ht="108.75" customHeight="1">
-      <c r="B42" s="48"/>
-      <c r="C42" s="41"/>
-      <c r="D42" s="34" t="s">
+      <c r="B42" s="28"/>
+      <c r="C42" s="34"/>
+      <c r="D42" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E42" s="22" t="s">
+      <c r="E42" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="F42" s="23"/>
+      <c r="F42" s="32"/>
     </row>
     <row r="43" spans="2:6" ht="32.25" customHeight="1">
-      <c r="B43" s="48"/>
-      <c r="C43" s="41"/>
-      <c r="D43" s="34" t="s">
+      <c r="B43" s="28"/>
+      <c r="C43" s="34"/>
+      <c r="D43" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E43" s="22" t="s">
+      <c r="E43" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="F43" s="23"/>
+      <c r="F43" s="32"/>
     </row>
     <row r="44" spans="2:6" ht="15" customHeight="1">
-      <c r="B44" s="48"/>
-      <c r="C44" s="41"/>
-      <c r="D44" s="34" t="s">
+      <c r="B44" s="28"/>
+      <c r="C44" s="34"/>
+      <c r="D44" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E44" s="22" t="s">
+      <c r="E44" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="F44" s="23"/>
+      <c r="F44" s="32"/>
     </row>
     <row r="45" spans="2:6" ht="15" customHeight="1">
-      <c r="B45" s="48"/>
-      <c r="C45" s="39" t="s">
+      <c r="B45" s="28"/>
+      <c r="C45" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="D45" s="45" t="s">
+      <c r="D45" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E45" s="24" t="s">
+      <c r="E45" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="F45" s="42"/>
+      <c r="F45" s="36"/>
     </row>
     <row r="46" spans="2:6" ht="30.75" customHeight="1">
-      <c r="B46" s="48"/>
-      <c r="C46" s="39"/>
-      <c r="D46" s="46"/>
-      <c r="E46" s="43"/>
-      <c r="F46" s="44"/>
+      <c r="B46" s="28"/>
+      <c r="C46" s="29"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="37"/>
+      <c r="F46" s="38"/>
     </row>
     <row r="47" spans="2:6" ht="13.5" customHeight="1"/>
     <row r="48" spans="2:6" ht="13.5" customHeight="1"/>
@@ -2310,19 +3411,11 @@
     <row r="60" ht="13.5" customHeight="1"/>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="B2:B46"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="C13:C40"/>
-    <mergeCell ref="D9:D12"/>
-    <mergeCell ref="C41:C44"/>
-    <mergeCell ref="E45:F46"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="D13:D20"/>
+    <mergeCell ref="E21:F26"/>
+    <mergeCell ref="E13:F20"/>
+    <mergeCell ref="D27:D29"/>
+    <mergeCell ref="E27:F29"/>
+    <mergeCell ref="E30:F30"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="E39:F39"/>
@@ -2332,15 +3425,1136 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E45:F46"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="B2:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="C13:C40"/>
+    <mergeCell ref="D9:D12"/>
+    <mergeCell ref="C41:C44"/>
+    <mergeCell ref="D13:D20"/>
     <mergeCell ref="C2:C12"/>
     <mergeCell ref="D21:D26"/>
-    <mergeCell ref="E21:F26"/>
-    <mergeCell ref="E13:F20"/>
-    <mergeCell ref="D27:D29"/>
-    <mergeCell ref="E27:F29"/>
-    <mergeCell ref="E30:F30"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:T160"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="6" max="6" width="18.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:20" ht="26.25" customHeight="1">
+      <c r="B2" s="70" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="70"/>
+      <c r="N2" s="70"/>
+      <c r="O2" s="70"/>
+      <c r="P2" s="70"/>
+      <c r="Q2" s="70"/>
+      <c r="R2" s="70"/>
+      <c r="S2" s="70"/>
+      <c r="T2" s="70"/>
+    </row>
+    <row r="3" spans="2:20" ht="13.5" customHeight="1">
+      <c r="B3" s="61" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="61"/>
+      <c r="L3" s="61"/>
+      <c r="M3" s="61"/>
+      <c r="N3" s="61"/>
+      <c r="O3" s="61"/>
+      <c r="P3" s="61"/>
+      <c r="Q3" s="61"/>
+      <c r="R3" s="61"/>
+      <c r="S3" s="61"/>
+      <c r="T3" s="61"/>
+    </row>
+    <row r="4" spans="2:20">
+      <c r="B4" s="61"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="61"/>
+      <c r="M4" s="61"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="61"/>
+      <c r="P4" s="61"/>
+      <c r="Q4" s="61"/>
+      <c r="R4" s="61"/>
+      <c r="S4" s="61"/>
+      <c r="T4" s="61"/>
+    </row>
+    <row r="5" spans="2:20" ht="29.25" customHeight="1">
+      <c r="B5" s="62"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="62"/>
+    </row>
+    <row r="6" spans="2:20">
+      <c r="B6" s="63" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="63"/>
+      <c r="K6" s="64" t="s">
+        <v>66</v>
+      </c>
+      <c r="L6" s="64"/>
+      <c r="M6" s="64"/>
+      <c r="N6" s="64"/>
+      <c r="O6" s="64"/>
+      <c r="P6" s="64"/>
+      <c r="Q6" s="64"/>
+      <c r="R6" s="64"/>
+      <c r="S6" s="64"/>
+      <c r="T6" s="64"/>
+    </row>
+    <row r="7" spans="2:20" ht="40.5" customHeight="1">
+      <c r="K7" s="61" t="s">
+        <v>67</v>
+      </c>
+      <c r="L7" s="61"/>
+      <c r="M7" s="61"/>
+      <c r="N7" s="61"/>
+      <c r="O7" s="61"/>
+      <c r="P7" s="61"/>
+      <c r="Q7" s="61"/>
+      <c r="R7" s="61"/>
+      <c r="S7" s="61"/>
+      <c r="T7" s="61"/>
+    </row>
+    <row r="8" spans="2:20">
+      <c r="K8" s="61"/>
+      <c r="L8" s="61"/>
+      <c r="M8" s="61"/>
+      <c r="N8" s="61"/>
+      <c r="O8" s="61"/>
+      <c r="P8" s="61"/>
+      <c r="Q8" s="61"/>
+      <c r="R8" s="61"/>
+      <c r="S8" s="61"/>
+      <c r="T8" s="61"/>
+    </row>
+    <row r="28" spans="2:20">
+      <c r="K28" s="55" t="s">
+        <v>68</v>
+      </c>
+      <c r="L28" s="55"/>
+      <c r="M28" s="55"/>
+      <c r="N28" s="55"/>
+      <c r="O28" s="55"/>
+      <c r="P28" s="55"/>
+      <c r="Q28" s="55"/>
+      <c r="R28" s="55"/>
+      <c r="S28" s="55"/>
+      <c r="T28" s="55"/>
+    </row>
+    <row r="29" spans="2:20">
+      <c r="K29" s="55"/>
+      <c r="L29" s="55"/>
+      <c r="M29" s="55"/>
+      <c r="N29" s="55"/>
+      <c r="O29" s="55"/>
+      <c r="P29" s="55"/>
+      <c r="Q29" s="55"/>
+      <c r="R29" s="55"/>
+      <c r="S29" s="55"/>
+      <c r="T29" s="55"/>
+    </row>
+    <row r="30" spans="2:20">
+      <c r="K30" s="55"/>
+      <c r="L30" s="55"/>
+      <c r="M30" s="55"/>
+      <c r="N30" s="55"/>
+      <c r="O30" s="55"/>
+      <c r="P30" s="55"/>
+      <c r="Q30" s="55"/>
+      <c r="R30" s="55"/>
+      <c r="S30" s="55"/>
+      <c r="T30" s="55"/>
+    </row>
+    <row r="31" spans="2:20">
+      <c r="K31" s="55"/>
+      <c r="L31" s="55"/>
+      <c r="M31" s="55"/>
+      <c r="N31" s="55"/>
+      <c r="O31" s="55"/>
+      <c r="P31" s="55"/>
+      <c r="Q31" s="55"/>
+      <c r="R31" s="55"/>
+      <c r="S31" s="55"/>
+      <c r="T31" s="55"/>
+    </row>
+    <row r="32" spans="2:20" ht="28.5" customHeight="1">
+      <c r="B32" s="57" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" s="57"/>
+      <c r="D32" s="57"/>
+      <c r="E32" s="57"/>
+      <c r="F32" s="57"/>
+      <c r="G32" s="57"/>
+      <c r="H32" s="57"/>
+      <c r="I32" s="57"/>
+      <c r="K32" s="55"/>
+      <c r="L32" s="55"/>
+      <c r="M32" s="55"/>
+      <c r="N32" s="55"/>
+      <c r="O32" s="55"/>
+      <c r="P32" s="55"/>
+      <c r="Q32" s="55"/>
+      <c r="R32" s="55"/>
+      <c r="S32" s="55"/>
+      <c r="T32" s="55"/>
+    </row>
+    <row r="33" spans="2:20">
+      <c r="K33" s="55"/>
+      <c r="L33" s="55"/>
+      <c r="M33" s="55"/>
+      <c r="N33" s="55"/>
+      <c r="O33" s="55"/>
+      <c r="P33" s="55"/>
+      <c r="Q33" s="55"/>
+      <c r="R33" s="55"/>
+      <c r="S33" s="55"/>
+      <c r="T33" s="55"/>
+    </row>
+    <row r="34" spans="2:20" ht="27" customHeight="1">
+      <c r="B34" s="56" t="s">
+        <v>56</v>
+      </c>
+      <c r="C34" s="56"/>
+      <c r="D34" s="56"/>
+      <c r="E34" s="56"/>
+      <c r="F34" s="56"/>
+      <c r="G34" s="56"/>
+      <c r="H34" s="56"/>
+      <c r="I34" s="56"/>
+      <c r="K34" s="55"/>
+      <c r="L34" s="55"/>
+      <c r="M34" s="55"/>
+      <c r="N34" s="55"/>
+      <c r="O34" s="55"/>
+      <c r="P34" s="55"/>
+      <c r="Q34" s="55"/>
+      <c r="R34" s="55"/>
+      <c r="S34" s="55"/>
+      <c r="T34" s="55"/>
+    </row>
+    <row r="35" spans="2:20">
+      <c r="K35" s="55"/>
+      <c r="L35" s="55"/>
+      <c r="M35" s="55"/>
+      <c r="N35" s="55"/>
+      <c r="O35" s="55"/>
+      <c r="P35" s="55"/>
+      <c r="Q35" s="55"/>
+      <c r="R35" s="55"/>
+      <c r="S35" s="55"/>
+      <c r="T35" s="55"/>
+    </row>
+    <row r="36" spans="2:20">
+      <c r="B36" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" s="56"/>
+      <c r="D36" s="56"/>
+      <c r="E36" s="56"/>
+      <c r="F36" s="56"/>
+      <c r="G36" s="56"/>
+      <c r="H36" s="56"/>
+      <c r="I36" s="56"/>
+    </row>
+    <row r="37" spans="2:20">
+      <c r="B37" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="C37" s="55"/>
+      <c r="D37" s="55"/>
+      <c r="E37" s="55"/>
+      <c r="F37" s="55"/>
+      <c r="G37" s="55"/>
+      <c r="H37" s="55"/>
+      <c r="I37" s="55"/>
+      <c r="J37" s="65"/>
+      <c r="K37" s="69" t="s">
+        <v>70</v>
+      </c>
+      <c r="L37" s="69"/>
+      <c r="M37" s="69"/>
+      <c r="N37" s="69"/>
+      <c r="O37" s="69"/>
+      <c r="P37" s="69"/>
+      <c r="Q37" s="69"/>
+      <c r="R37" s="69"/>
+      <c r="S37" s="69"/>
+      <c r="T37" s="69"/>
+    </row>
+    <row r="38" spans="2:20">
+      <c r="B38" s="55"/>
+      <c r="C38" s="55"/>
+      <c r="D38" s="55"/>
+      <c r="E38" s="55"/>
+      <c r="F38" s="55"/>
+      <c r="G38" s="55"/>
+      <c r="H38" s="55"/>
+      <c r="I38" s="55"/>
+      <c r="J38" s="65"/>
+      <c r="K38" s="69"/>
+      <c r="L38" s="69"/>
+      <c r="M38" s="69"/>
+      <c r="N38" s="69"/>
+      <c r="O38" s="69"/>
+      <c r="P38" s="69"/>
+      <c r="Q38" s="69"/>
+      <c r="R38" s="69"/>
+      <c r="S38" s="69"/>
+      <c r="T38" s="69"/>
+    </row>
+    <row r="39" spans="2:20">
+      <c r="B39" s="55"/>
+      <c r="C39" s="55"/>
+      <c r="D39" s="55"/>
+      <c r="E39" s="55"/>
+      <c r="F39" s="55"/>
+      <c r="G39" s="55"/>
+      <c r="H39" s="55"/>
+      <c r="I39" s="55"/>
+      <c r="J39" s="65"/>
+    </row>
+    <row r="40" spans="2:20">
+      <c r="B40" s="55"/>
+      <c r="C40" s="55"/>
+      <c r="D40" s="55"/>
+      <c r="E40" s="55"/>
+      <c r="F40" s="55"/>
+      <c r="G40" s="55"/>
+      <c r="H40" s="55"/>
+      <c r="I40" s="55"/>
+      <c r="J40" s="65"/>
+      <c r="K40" s="68" t="s">
+        <v>69</v>
+      </c>
+      <c r="L40" s="68"/>
+      <c r="M40" s="68"/>
+      <c r="N40" s="68"/>
+      <c r="O40" s="68"/>
+      <c r="P40" s="68"/>
+      <c r="Q40" s="68"/>
+      <c r="R40" s="68"/>
+      <c r="S40" s="68"/>
+      <c r="T40" s="68"/>
+    </row>
+    <row r="41" spans="2:20">
+      <c r="B41" s="55"/>
+      <c r="C41" s="55"/>
+      <c r="D41" s="55"/>
+      <c r="E41" s="55"/>
+      <c r="F41" s="55"/>
+      <c r="G41" s="55"/>
+      <c r="H41" s="55"/>
+      <c r="I41" s="55"/>
+      <c r="J41" s="65"/>
+    </row>
+    <row r="42" spans="2:20">
+      <c r="B42" s="55"/>
+      <c r="C42" s="55"/>
+      <c r="D42" s="55"/>
+      <c r="E42" s="55"/>
+      <c r="F42" s="55"/>
+      <c r="G42" s="55"/>
+      <c r="H42" s="55"/>
+      <c r="I42" s="55"/>
+      <c r="J42" s="65"/>
+    </row>
+    <row r="43" spans="2:20">
+      <c r="B43" s="55"/>
+      <c r="C43" s="55"/>
+      <c r="D43" s="55"/>
+      <c r="E43" s="55"/>
+      <c r="F43" s="55"/>
+      <c r="G43" s="55"/>
+      <c r="H43" s="55"/>
+      <c r="I43" s="55"/>
+      <c r="J43" s="65"/>
+    </row>
+    <row r="44" spans="2:20">
+      <c r="B44" s="55"/>
+      <c r="C44" s="55"/>
+      <c r="D44" s="55"/>
+      <c r="E44" s="55"/>
+      <c r="F44" s="55"/>
+      <c r="G44" s="55"/>
+      <c r="H44" s="55"/>
+      <c r="I44" s="55"/>
+      <c r="J44" s="65"/>
+    </row>
+    <row r="46" spans="2:20">
+      <c r="B46" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="C46" s="39"/>
+      <c r="D46" s="58" t="s">
+        <v>59</v>
+      </c>
+      <c r="E46" s="32"/>
+      <c r="F46" s="32"/>
+      <c r="G46" s="32"/>
+      <c r="H46" s="32"/>
+      <c r="I46" s="32"/>
+      <c r="J46" s="66"/>
+    </row>
+    <row r="47" spans="2:20">
+      <c r="B47" s="39"/>
+      <c r="C47" s="39"/>
+      <c r="D47" s="59" t="s">
+        <v>60</v>
+      </c>
+      <c r="E47" s="39"/>
+      <c r="F47" s="39"/>
+      <c r="G47" s="39"/>
+      <c r="H47" s="39"/>
+      <c r="I47" s="39"/>
+      <c r="J47" s="67"/>
+    </row>
+    <row r="48" spans="2:20">
+      <c r="B48" s="39"/>
+      <c r="C48" s="39"/>
+      <c r="D48" s="59"/>
+      <c r="E48" s="39"/>
+      <c r="F48" s="39"/>
+      <c r="G48" s="39"/>
+      <c r="H48" s="39"/>
+      <c r="I48" s="39"/>
+      <c r="J48" s="67"/>
+    </row>
+    <row r="49" spans="2:20">
+      <c r="B49" s="39"/>
+      <c r="C49" s="39"/>
+      <c r="D49" s="59"/>
+      <c r="E49" s="39"/>
+      <c r="F49" s="39"/>
+      <c r="G49" s="39"/>
+      <c r="H49" s="39"/>
+      <c r="I49" s="39"/>
+      <c r="J49" s="67"/>
+    </row>
+    <row r="50" spans="2:20">
+      <c r="B50" s="39"/>
+      <c r="C50" s="39"/>
+      <c r="D50" s="59" t="s">
+        <v>61</v>
+      </c>
+      <c r="E50" s="39"/>
+      <c r="F50" s="39"/>
+      <c r="G50" s="39"/>
+      <c r="H50" s="39"/>
+      <c r="I50" s="39"/>
+      <c r="J50" s="67"/>
+    </row>
+    <row r="51" spans="2:20">
+      <c r="B51" s="39"/>
+      <c r="C51" s="39"/>
+      <c r="D51" s="59"/>
+      <c r="E51" s="39"/>
+      <c r="F51" s="39"/>
+      <c r="G51" s="39"/>
+      <c r="H51" s="39"/>
+      <c r="I51" s="39"/>
+      <c r="J51" s="67"/>
+    </row>
+    <row r="52" spans="2:20">
+      <c r="B52" s="39"/>
+      <c r="C52" s="39"/>
+    </row>
+    <row r="53" spans="2:20">
+      <c r="B53" s="39"/>
+      <c r="C53" s="39"/>
+      <c r="D53" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="E53" s="39"/>
+      <c r="F53" s="39"/>
+      <c r="G53" s="39"/>
+      <c r="H53" s="39"/>
+      <c r="I53" s="39"/>
+      <c r="J53" s="67"/>
+    </row>
+    <row r="54" spans="2:20">
+      <c r="B54" s="39"/>
+      <c r="C54" s="39"/>
+      <c r="D54" s="39"/>
+      <c r="E54" s="39"/>
+      <c r="F54" s="39"/>
+      <c r="G54" s="39"/>
+      <c r="H54" s="39"/>
+      <c r="I54" s="39"/>
+      <c r="J54" s="67"/>
+    </row>
+    <row r="64" spans="2:20" ht="28.5" customHeight="1">
+      <c r="B64" s="70" t="s">
+        <v>77</v>
+      </c>
+      <c r="C64" s="70"/>
+      <c r="D64" s="70"/>
+      <c r="E64" s="70"/>
+      <c r="F64" s="70"/>
+      <c r="G64" s="70"/>
+      <c r="H64" s="70"/>
+      <c r="I64" s="70"/>
+      <c r="J64" s="70"/>
+      <c r="K64" s="70"/>
+      <c r="L64" s="70"/>
+      <c r="M64" s="70"/>
+      <c r="N64" s="70"/>
+      <c r="O64" s="70"/>
+      <c r="P64" s="70"/>
+      <c r="Q64" s="70"/>
+      <c r="R64" s="70"/>
+      <c r="S64" s="70"/>
+      <c r="T64" s="70"/>
+    </row>
+    <row r="65" spans="2:20" ht="13.5" customHeight="1"/>
+    <row r="66" spans="2:20" ht="0.75" customHeight="1"/>
+    <row r="67" spans="2:20">
+      <c r="B67" s="63" t="s">
+        <v>65</v>
+      </c>
+      <c r="C67" s="63"/>
+      <c r="D67" s="63"/>
+      <c r="E67" s="63"/>
+      <c r="F67" s="63"/>
+      <c r="G67" s="63"/>
+      <c r="H67" s="63"/>
+      <c r="I67" s="63"/>
+      <c r="K67" s="64" t="s">
+        <v>66</v>
+      </c>
+      <c r="L67" s="64"/>
+      <c r="M67" s="64"/>
+      <c r="N67" s="64"/>
+      <c r="O67" s="64"/>
+      <c r="P67" s="64"/>
+      <c r="Q67" s="64"/>
+      <c r="R67" s="64"/>
+      <c r="S67" s="64"/>
+      <c r="T67" s="64"/>
+    </row>
+    <row r="69" spans="2:20">
+      <c r="K69" s="55" t="s">
+        <v>71</v>
+      </c>
+      <c r="L69" s="55"/>
+      <c r="M69" s="55"/>
+      <c r="N69" s="55"/>
+      <c r="O69" s="55"/>
+      <c r="P69" s="55"/>
+      <c r="Q69" s="55"/>
+      <c r="R69" s="55"/>
+      <c r="S69" s="55"/>
+      <c r="T69" s="55"/>
+    </row>
+    <row r="70" spans="2:20" ht="13.5" customHeight="1"/>
+    <row r="71" spans="2:20" ht="13.5" customHeight="1">
+      <c r="K71" s="55" t="s">
+        <v>72</v>
+      </c>
+      <c r="L71" s="55"/>
+      <c r="M71" s="55"/>
+      <c r="N71" s="55"/>
+      <c r="O71" s="55"/>
+      <c r="P71" s="55"/>
+      <c r="Q71" s="55"/>
+      <c r="R71" s="55"/>
+      <c r="S71" s="55"/>
+      <c r="T71" s="55"/>
+    </row>
+    <row r="72" spans="2:20">
+      <c r="K72" s="55"/>
+      <c r="L72" s="55"/>
+      <c r="M72" s="55"/>
+      <c r="N72" s="55"/>
+      <c r="O72" s="55"/>
+      <c r="P72" s="55"/>
+      <c r="Q72" s="55"/>
+      <c r="R72" s="55"/>
+      <c r="S72" s="55"/>
+      <c r="T72" s="55"/>
+    </row>
+    <row r="73" spans="2:20" ht="34.5" customHeight="1">
+      <c r="K73" s="55"/>
+      <c r="L73" s="55"/>
+      <c r="M73" s="55"/>
+      <c r="N73" s="55"/>
+      <c r="O73" s="55"/>
+      <c r="P73" s="55"/>
+      <c r="Q73" s="55"/>
+      <c r="R73" s="55"/>
+      <c r="S73" s="55"/>
+      <c r="T73" s="55"/>
+    </row>
+    <row r="75" spans="2:20">
+      <c r="K75" s="55" t="s">
+        <v>73</v>
+      </c>
+      <c r="L75" s="55"/>
+      <c r="M75" s="55"/>
+      <c r="N75" s="55"/>
+      <c r="O75" s="55"/>
+      <c r="P75" s="55"/>
+      <c r="Q75" s="55"/>
+      <c r="R75" s="55"/>
+      <c r="S75" s="55"/>
+      <c r="T75" s="55"/>
+    </row>
+    <row r="76" spans="2:20" ht="49.5" customHeight="1">
+      <c r="K76" s="55"/>
+      <c r="L76" s="55"/>
+      <c r="M76" s="55"/>
+      <c r="N76" s="55"/>
+      <c r="O76" s="55"/>
+      <c r="P76" s="55"/>
+      <c r="Q76" s="55"/>
+      <c r="R76" s="55"/>
+      <c r="S76" s="55"/>
+      <c r="T76" s="55"/>
+    </row>
+    <row r="78" spans="2:20" ht="42.75" customHeight="1">
+      <c r="B78" s="55" t="s">
+        <v>75</v>
+      </c>
+      <c r="C78" s="55"/>
+      <c r="D78" s="55"/>
+      <c r="E78" s="55"/>
+      <c r="F78" s="55"/>
+      <c r="G78" s="55"/>
+      <c r="H78" s="55"/>
+      <c r="I78" s="55"/>
+      <c r="K78" s="55" t="s">
+        <v>74</v>
+      </c>
+      <c r="L78" s="55"/>
+      <c r="M78" s="55"/>
+      <c r="N78" s="55"/>
+      <c r="O78" s="55"/>
+      <c r="P78" s="55"/>
+      <c r="Q78" s="55"/>
+      <c r="R78" s="55"/>
+      <c r="S78" s="55"/>
+      <c r="T78" s="55"/>
+    </row>
+    <row r="80" spans="2:20" ht="27" customHeight="1">
+      <c r="B80" s="70" t="s">
+        <v>76</v>
+      </c>
+      <c r="C80" s="70"/>
+      <c r="D80" s="70"/>
+      <c r="E80" s="70"/>
+      <c r="F80" s="70"/>
+      <c r="G80" s="70"/>
+      <c r="H80" s="70"/>
+      <c r="I80" s="70"/>
+      <c r="J80" s="70"/>
+      <c r="K80" s="70"/>
+      <c r="L80" s="70"/>
+      <c r="M80" s="70"/>
+      <c r="N80" s="70"/>
+      <c r="O80" s="70"/>
+      <c r="P80" s="70"/>
+      <c r="Q80" s="70"/>
+      <c r="R80" s="70"/>
+      <c r="S80" s="70"/>
+      <c r="T80" s="70"/>
+    </row>
+    <row r="81" spans="2:20" ht="67.5" customHeight="1">
+      <c r="B81" s="55" t="s">
+        <v>78</v>
+      </c>
+      <c r="C81" s="55"/>
+      <c r="D81" s="55"/>
+      <c r="E81" s="55"/>
+      <c r="F81" s="55"/>
+      <c r="G81" s="55"/>
+      <c r="H81" s="55"/>
+      <c r="I81" s="55"/>
+      <c r="J81" s="55"/>
+      <c r="K81" s="55"/>
+      <c r="L81" s="55"/>
+      <c r="M81" s="55"/>
+      <c r="N81" s="55"/>
+      <c r="O81" s="55"/>
+      <c r="P81" s="55"/>
+      <c r="Q81" s="55"/>
+      <c r="R81" s="55"/>
+      <c r="S81" s="55"/>
+      <c r="T81" s="55"/>
+    </row>
+    <row r="83" spans="2:20">
+      <c r="B83" s="63" t="s">
+        <v>65</v>
+      </c>
+      <c r="C83" s="63"/>
+      <c r="D83" s="63"/>
+      <c r="E83" s="63"/>
+      <c r="F83" s="63"/>
+      <c r="G83" s="63"/>
+      <c r="H83" s="63"/>
+      <c r="I83" s="63"/>
+      <c r="K83" s="64" t="s">
+        <v>66</v>
+      </c>
+      <c r="L83" s="64"/>
+      <c r="M83" s="64"/>
+      <c r="N83" s="64"/>
+      <c r="O83" s="64"/>
+      <c r="P83" s="64"/>
+      <c r="Q83" s="64"/>
+      <c r="R83" s="64"/>
+      <c r="S83" s="64"/>
+      <c r="T83" s="64"/>
+    </row>
+    <row r="85" spans="2:20">
+      <c r="K85" s="55" t="s">
+        <v>82</v>
+      </c>
+      <c r="L85" s="55"/>
+      <c r="M85" s="55"/>
+      <c r="N85" s="55"/>
+      <c r="O85" s="55"/>
+      <c r="P85" s="55"/>
+      <c r="Q85" s="55"/>
+      <c r="R85" s="55"/>
+      <c r="S85" s="55"/>
+      <c r="T85" s="55"/>
+    </row>
+    <row r="86" spans="2:20" ht="40.5" customHeight="1">
+      <c r="K86" s="55"/>
+      <c r="L86" s="55"/>
+      <c r="M86" s="55"/>
+      <c r="N86" s="55"/>
+      <c r="O86" s="55"/>
+      <c r="P86" s="55"/>
+      <c r="Q86" s="55"/>
+      <c r="R86" s="55"/>
+      <c r="S86" s="55"/>
+      <c r="T86" s="55"/>
+    </row>
+    <row r="100" spans="2:20" ht="13.5" customHeight="1">
+      <c r="B100" s="55" t="s">
+        <v>79</v>
+      </c>
+      <c r="C100" s="55"/>
+      <c r="D100" s="55"/>
+      <c r="E100" s="55"/>
+      <c r="F100" s="55"/>
+      <c r="G100" s="55"/>
+      <c r="H100" s="55"/>
+      <c r="I100" s="55"/>
+      <c r="J100" s="60"/>
+      <c r="K100" s="60"/>
+    </row>
+    <row r="101" spans="2:20">
+      <c r="B101" s="55"/>
+      <c r="C101" s="55"/>
+      <c r="D101" s="55"/>
+      <c r="E101" s="55"/>
+      <c r="F101" s="55"/>
+      <c r="G101" s="55"/>
+      <c r="H101" s="55"/>
+      <c r="I101" s="55"/>
+      <c r="J101" s="60"/>
+      <c r="K101" s="60"/>
+    </row>
+    <row r="102" spans="2:20">
+      <c r="B102" s="55"/>
+      <c r="C102" s="55"/>
+      <c r="D102" s="55"/>
+      <c r="E102" s="55"/>
+      <c r="F102" s="55"/>
+      <c r="G102" s="55"/>
+      <c r="H102" s="55"/>
+      <c r="I102" s="55"/>
+    </row>
+    <row r="103" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B103" s="55"/>
+      <c r="C103" s="55"/>
+      <c r="D103" s="55"/>
+      <c r="E103" s="55"/>
+      <c r="F103" s="55"/>
+      <c r="G103" s="55"/>
+      <c r="H103" s="55"/>
+      <c r="I103" s="55"/>
+    </row>
+    <row r="105" spans="2:20" ht="27" customHeight="1">
+      <c r="B105" s="55" t="s">
+        <v>80</v>
+      </c>
+      <c r="C105" s="55"/>
+      <c r="D105" s="55"/>
+      <c r="E105" s="55"/>
+      <c r="F105" s="55"/>
+      <c r="G105" s="55"/>
+      <c r="H105" s="55"/>
+      <c r="I105" s="55"/>
+      <c r="K105" s="55" t="s">
+        <v>83</v>
+      </c>
+      <c r="L105" s="55"/>
+      <c r="M105" s="55"/>
+      <c r="N105" s="55"/>
+      <c r="O105" s="55"/>
+      <c r="P105" s="55"/>
+      <c r="Q105" s="55"/>
+      <c r="R105" s="55"/>
+      <c r="S105" s="55"/>
+      <c r="T105" s="55"/>
+    </row>
+    <row r="106" spans="2:20" ht="27.75" customHeight="1">
+      <c r="B106" s="55"/>
+      <c r="C106" s="55"/>
+      <c r="D106" s="55"/>
+      <c r="E106" s="55"/>
+      <c r="F106" s="55"/>
+      <c r="G106" s="55"/>
+      <c r="H106" s="55"/>
+      <c r="I106" s="55"/>
+      <c r="K106" s="55"/>
+      <c r="L106" s="55"/>
+      <c r="M106" s="55"/>
+      <c r="N106" s="55"/>
+      <c r="O106" s="55"/>
+      <c r="P106" s="55"/>
+      <c r="Q106" s="55"/>
+      <c r="R106" s="55"/>
+      <c r="S106" s="55"/>
+      <c r="T106" s="55"/>
+    </row>
+    <row r="108" spans="2:20" ht="27.75" customHeight="1">
+      <c r="B108" s="55" t="s">
+        <v>81</v>
+      </c>
+      <c r="C108" s="55"/>
+      <c r="D108" s="55"/>
+      <c r="E108" s="55"/>
+      <c r="F108" s="55"/>
+      <c r="G108" s="55"/>
+      <c r="H108" s="55"/>
+      <c r="I108" s="55"/>
+      <c r="K108" s="55" t="s">
+        <v>84</v>
+      </c>
+      <c r="L108" s="55"/>
+      <c r="M108" s="55"/>
+      <c r="N108" s="55"/>
+      <c r="O108" s="55"/>
+      <c r="P108" s="55"/>
+      <c r="Q108" s="55"/>
+      <c r="R108" s="55"/>
+      <c r="S108" s="55"/>
+      <c r="T108" s="55"/>
+    </row>
+    <row r="109" spans="2:20" ht="27.75" customHeight="1">
+      <c r="B109" s="55"/>
+      <c r="C109" s="55"/>
+      <c r="D109" s="55"/>
+      <c r="E109" s="55"/>
+      <c r="F109" s="55"/>
+      <c r="G109" s="55"/>
+      <c r="H109" s="55"/>
+      <c r="I109" s="55"/>
+      <c r="K109" s="55"/>
+      <c r="L109" s="55"/>
+      <c r="M109" s="55"/>
+      <c r="N109" s="55"/>
+      <c r="O109" s="55"/>
+      <c r="P109" s="55"/>
+      <c r="Q109" s="55"/>
+      <c r="R109" s="55"/>
+      <c r="S109" s="55"/>
+      <c r="T109" s="55"/>
+    </row>
+    <row r="110" spans="2:20" ht="40.5" customHeight="1">
+      <c r="B110" s="55"/>
+      <c r="C110" s="55"/>
+      <c r="D110" s="55"/>
+      <c r="E110" s="55"/>
+      <c r="F110" s="55"/>
+      <c r="G110" s="55"/>
+      <c r="H110" s="55"/>
+      <c r="I110" s="55"/>
+      <c r="K110" s="55"/>
+      <c r="L110" s="55"/>
+      <c r="M110" s="55"/>
+      <c r="N110" s="55"/>
+      <c r="O110" s="55"/>
+      <c r="P110" s="55"/>
+      <c r="Q110" s="55"/>
+      <c r="R110" s="55"/>
+      <c r="S110" s="55"/>
+      <c r="T110" s="55"/>
+    </row>
+    <row r="112" spans="2:20">
+      <c r="K112" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="L112" s="55"/>
+      <c r="M112" s="55"/>
+      <c r="N112" s="55"/>
+      <c r="O112" s="55"/>
+      <c r="P112" s="55"/>
+      <c r="Q112" s="55"/>
+      <c r="R112" s="55"/>
+      <c r="S112" s="55"/>
+      <c r="T112" s="55"/>
+    </row>
+    <row r="149" spans="2:20" ht="53.25" customHeight="1">
+      <c r="K149" s="55" t="s">
+        <v>86</v>
+      </c>
+      <c r="L149" s="55"/>
+      <c r="M149" s="55"/>
+      <c r="N149" s="55"/>
+      <c r="O149" s="55"/>
+      <c r="P149" s="55"/>
+      <c r="Q149" s="55"/>
+      <c r="R149" s="55"/>
+      <c r="S149" s="55"/>
+      <c r="T149" s="55"/>
+    </row>
+    <row r="150" spans="2:20" ht="40.5" customHeight="1">
+      <c r="K150" s="55"/>
+      <c r="L150" s="55"/>
+      <c r="M150" s="55"/>
+      <c r="N150" s="55"/>
+      <c r="O150" s="55"/>
+      <c r="P150" s="55"/>
+      <c r="Q150" s="55"/>
+      <c r="R150" s="55"/>
+      <c r="S150" s="55"/>
+      <c r="T150" s="55"/>
+    </row>
+    <row r="151" spans="2:20" ht="41.25" customHeight="1">
+      <c r="K151" s="55"/>
+      <c r="L151" s="55"/>
+      <c r="M151" s="55"/>
+      <c r="N151" s="55"/>
+      <c r="O151" s="55"/>
+      <c r="P151" s="55"/>
+      <c r="Q151" s="55"/>
+      <c r="R151" s="55"/>
+      <c r="S151" s="55"/>
+      <c r="T151" s="55"/>
+    </row>
+    <row r="152" spans="2:20">
+      <c r="K152" s="55"/>
+      <c r="L152" s="55"/>
+      <c r="M152" s="55"/>
+      <c r="N152" s="55"/>
+      <c r="O152" s="55"/>
+      <c r="P152" s="55"/>
+      <c r="Q152" s="55"/>
+      <c r="R152" s="55"/>
+      <c r="S152" s="55"/>
+      <c r="T152" s="55"/>
+    </row>
+    <row r="153" spans="2:20" ht="54" customHeight="1">
+      <c r="K153" s="55"/>
+      <c r="L153" s="55"/>
+      <c r="M153" s="55"/>
+      <c r="N153" s="55"/>
+      <c r="O153" s="55"/>
+      <c r="P153" s="55"/>
+      <c r="Q153" s="55"/>
+      <c r="R153" s="55"/>
+      <c r="S153" s="55"/>
+      <c r="T153" s="55"/>
+    </row>
+    <row r="155" spans="2:20">
+      <c r="K155" s="55" t="s">
+        <v>87</v>
+      </c>
+      <c r="L155" s="55"/>
+      <c r="M155" s="55"/>
+      <c r="N155" s="55"/>
+      <c r="O155" s="55"/>
+      <c r="P155" s="55"/>
+      <c r="Q155" s="55"/>
+      <c r="R155" s="55"/>
+      <c r="S155" s="55"/>
+      <c r="T155" s="55"/>
+    </row>
+    <row r="156" spans="2:20" ht="27" customHeight="1">
+      <c r="K156" s="55"/>
+      <c r="L156" s="55"/>
+      <c r="M156" s="55"/>
+      <c r="N156" s="55"/>
+      <c r="O156" s="55"/>
+      <c r="P156" s="55"/>
+      <c r="Q156" s="55"/>
+      <c r="R156" s="55"/>
+      <c r="S156" s="55"/>
+      <c r="T156" s="55"/>
+    </row>
+    <row r="158" spans="2:20">
+      <c r="B158" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="C158" s="70"/>
+      <c r="D158" s="70"/>
+      <c r="E158" s="70"/>
+      <c r="F158" s="70"/>
+      <c r="G158" s="70"/>
+      <c r="H158" s="70"/>
+      <c r="I158" s="70"/>
+      <c r="J158" s="70"/>
+      <c r="K158" s="70"/>
+      <c r="L158" s="70"/>
+      <c r="M158" s="70"/>
+      <c r="N158" s="70"/>
+      <c r="O158" s="70"/>
+      <c r="P158" s="70"/>
+      <c r="Q158" s="70"/>
+      <c r="R158" s="70"/>
+      <c r="S158" s="70"/>
+      <c r="T158" s="70"/>
+    </row>
+    <row r="159" spans="2:20" ht="26.25" customHeight="1">
+      <c r="B159" s="55" t="s">
+        <v>89</v>
+      </c>
+      <c r="C159" s="55"/>
+      <c r="D159" s="55"/>
+      <c r="E159" s="55"/>
+      <c r="F159" s="55"/>
+      <c r="G159" s="55"/>
+      <c r="H159" s="55"/>
+      <c r="I159" s="55"/>
+      <c r="J159" s="55"/>
+      <c r="K159" s="55"/>
+      <c r="L159" s="55"/>
+      <c r="M159" s="55"/>
+      <c r="N159" s="55"/>
+      <c r="O159" s="55"/>
+      <c r="P159" s="55"/>
+      <c r="Q159" s="55"/>
+      <c r="R159" s="55"/>
+      <c r="S159" s="55"/>
+      <c r="T159" s="55"/>
+    </row>
+    <row r="160" spans="2:20" ht="39.75" customHeight="1">
+      <c r="B160" s="55"/>
+      <c r="C160" s="55"/>
+      <c r="D160" s="55"/>
+      <c r="E160" s="55"/>
+      <c r="F160" s="55"/>
+      <c r="G160" s="55"/>
+      <c r="H160" s="55"/>
+      <c r="I160" s="55"/>
+      <c r="J160" s="55"/>
+      <c r="K160" s="55"/>
+      <c r="L160" s="55"/>
+      <c r="M160" s="55"/>
+      <c r="N160" s="55"/>
+      <c r="O160" s="55"/>
+      <c r="P160" s="55"/>
+      <c r="Q160" s="55"/>
+      <c r="R160" s="55"/>
+      <c r="S160" s="55"/>
+      <c r="T160" s="55"/>
+    </row>
+  </sheetData>
+  <mergeCells count="40">
+    <mergeCell ref="K149:T153"/>
+    <mergeCell ref="K155:T156"/>
+    <mergeCell ref="B158:T158"/>
+    <mergeCell ref="B159:T160"/>
+    <mergeCell ref="B105:I106"/>
+    <mergeCell ref="B108:I110"/>
+    <mergeCell ref="K105:T106"/>
+    <mergeCell ref="K108:T110"/>
+    <mergeCell ref="K112:T112"/>
+    <mergeCell ref="B80:T80"/>
+    <mergeCell ref="B83:I83"/>
+    <mergeCell ref="K83:T83"/>
+    <mergeCell ref="B81:T81"/>
+    <mergeCell ref="K85:T86"/>
+    <mergeCell ref="B100:I103"/>
+    <mergeCell ref="K75:T76"/>
+    <mergeCell ref="K78:T78"/>
+    <mergeCell ref="B64:T64"/>
+    <mergeCell ref="B67:I67"/>
+    <mergeCell ref="K67:T67"/>
+    <mergeCell ref="B78:I78"/>
+    <mergeCell ref="K28:T35"/>
+    <mergeCell ref="K40:T40"/>
+    <mergeCell ref="K37:T38"/>
+    <mergeCell ref="K69:T69"/>
+    <mergeCell ref="K71:T73"/>
+    <mergeCell ref="K6:T6"/>
+    <mergeCell ref="K7:T8"/>
+    <mergeCell ref="B3:T4"/>
+    <mergeCell ref="B2:T2"/>
+    <mergeCell ref="B32:I32"/>
+    <mergeCell ref="B34:I34"/>
+    <mergeCell ref="B36:I36"/>
+    <mergeCell ref="B37:I44"/>
+    <mergeCell ref="B46:C54"/>
+    <mergeCell ref="D46:I46"/>
+    <mergeCell ref="D47:I49"/>
+    <mergeCell ref="D50:I51"/>
+    <mergeCell ref="D53:I54"/>
+    <mergeCell ref="B6:I6"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>